<commit_message>
Enhance Cutting Optimizer Pro: - Update .gitignore to include additional files and directories. - Modify Cutting-Optimizer-Pro.spec to include hidden imports and change the application icon path. - Implement logging functionality in gui.py for better error tracking and debugging. - Add update checking feature with user notifications in gui.py. - Update translations.json for new update-related messages. - Update version.json to 1.1.0. - Replace old icons with new dark/light theme icons. - Update README.md with new screenshots and contact information. - Remove unused icon files to clean up the project.
</commit_message>
<xml_diff>
--- a/optimized_cutting_plan.xlsx
+++ b/optimized_cutting_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="173">
   <si>
     <t>Profile</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Remaining Length</t>
   </si>
   <si>
+    <t>nan</t>
+  </si>
+  <si>
     <t>HEA140</t>
   </si>
   <si>
@@ -223,10 +226,7 @@
     <t>UPN200</t>
   </si>
   <si>
-    <t>ADE</t>
-  </si>
-  <si>
-    <t>ADEZ</t>
+    <t>[0, 0, 0, 0]</t>
   </si>
   <si>
     <t>[1435, 1435]</t>
@@ -533,12 +533,6 @@
   </si>
   <si>
     <t>[1200, 1200, 1200, 1200]</t>
-  </si>
-  <si>
-    <t>[4500]</t>
-  </si>
-  <si>
-    <t>[1500, 1500, 1500]</t>
   </si>
 </sst>
 </file>
@@ -623,8 +617,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>18</xdr:colOff>
-      <xdr:row>625</xdr:row>
-      <xdr:rowOff>238</xdr:rowOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>76434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -642,7 +636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4267200" y="190500"/>
-          <a:ext cx="9144018" cy="118872238"/>
+          <a:ext cx="9144018" cy="117043434"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -939,7 +933,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -976,13 +970,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2">
-        <v>2870</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2870</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -996,44 +990,44 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3">
-        <v>11962</v>
+        <v>2870</v>
       </c>
       <c r="F3">
-        <v>11962</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>12000</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4">
-        <v>11924</v>
+        <v>11962</v>
       </c>
       <c r="F4">
-        <v>11924</v>
+        <v>11962</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>12000</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>73</v>
@@ -1047,22 +1041,22 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>12000</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6">
-        <v>8886</v>
+        <v>11924</v>
       </c>
       <c r="F6">
-        <v>8886</v>
+        <v>11924</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1073,27 +1067,27 @@
         <v>12000</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E7">
-        <v>11924</v>
+        <v>8886</v>
       </c>
       <c r="F7">
-        <v>11924</v>
+        <v>8886</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>12000</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>73</v>
@@ -1107,13 +1101,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>12000</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -1127,13 +1121,13 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>12000</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>73</v>
@@ -1147,22 +1141,22 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>12000</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11">
-        <v>11848</v>
+        <v>11924</v>
       </c>
       <c r="F11">
-        <v>11848</v>
+        <v>11924</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1173,27 +1167,27 @@
         <v>12000</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12">
-        <v>6579</v>
+        <v>11848</v>
       </c>
       <c r="F12">
-        <v>6579</v>
+        <v>11848</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>12000</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>76</v>
@@ -1207,13 +1201,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>12000</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>76</v>
@@ -1227,13 +1221,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>12000</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
         <v>76</v>
@@ -1247,13 +1241,13 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>12000</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>76</v>
@@ -1267,13 +1261,13 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>12000</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>76</v>
@@ -1287,13 +1281,13 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>12000</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
         <v>76</v>
@@ -1307,13 +1301,13 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>12000</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
         <v>76</v>
@@ -1327,33 +1321,33 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>12000</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20">
-        <v>11940</v>
+        <v>6579</v>
       </c>
       <c r="F20">
-        <v>11940</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>12000</v>
+      </c>
+      <c r="C21">
         <v>9</v>
-      </c>
-      <c r="B21">
-        <v>12000</v>
-      </c>
-      <c r="C21">
-        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>77</v>
@@ -1367,13 +1361,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>12000</v>
       </c>
       <c r="C22">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>77</v>
@@ -1387,13 +1381,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23">
         <v>12000</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
         <v>77</v>
@@ -1413,27 +1407,27 @@
         <v>12000</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24">
-        <v>6130</v>
+        <v>11940</v>
       </c>
       <c r="F24">
-        <v>6130</v>
+        <v>11940</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25">
         <v>12000</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>78</v>
@@ -1447,13 +1441,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B26">
         <v>12000</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>78</v>
@@ -1467,13 +1461,13 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B27">
         <v>12000</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
         <v>78</v>
@@ -1487,13 +1481,13 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28">
         <v>12000</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>78</v>
@@ -1507,13 +1501,13 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29">
         <v>12000</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
         <v>78</v>
@@ -1527,13 +1521,13 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>12000</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" t="s">
         <v>78</v>
@@ -1547,13 +1541,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31">
         <v>12000</v>
       </c>
       <c r="C31">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>78</v>
@@ -1567,13 +1561,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32">
         <v>12000</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
         <v>78</v>
@@ -1587,13 +1581,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>12000</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
         <v>78</v>
@@ -1607,13 +1601,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>12000</v>
+      </c>
+      <c r="C34">
         <v>10</v>
-      </c>
-      <c r="B34">
-        <v>12000</v>
-      </c>
-      <c r="C34">
-        <v>11</v>
       </c>
       <c r="D34" t="s">
         <v>78</v>
@@ -1627,13 +1621,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>12000</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
         <v>78</v>
@@ -1647,13 +1641,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>12000</v>
       </c>
       <c r="C36">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
         <v>78</v>
@@ -1667,13 +1661,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>12000</v>
       </c>
       <c r="C37">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
         <v>78</v>
@@ -1687,33 +1681,33 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>12000</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38">
-        <v>11980</v>
+        <v>6130</v>
       </c>
       <c r="F38">
-        <v>11980</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>12000</v>
       </c>
       <c r="C39">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
         <v>79</v>
@@ -1727,13 +1721,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>12000</v>
       </c>
       <c r="C40">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>79</v>
@@ -1747,13 +1741,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>12000</v>
       </c>
       <c r="C41">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
         <v>79</v>
@@ -1767,13 +1761,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>12000</v>
       </c>
       <c r="C42">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
         <v>79</v>
@@ -1787,13 +1781,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>12000</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" t="s">
         <v>79</v>
@@ -1807,13 +1801,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>12000</v>
       </c>
       <c r="C44">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
         <v>79</v>
@@ -1827,33 +1821,33 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>12000</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E45">
-        <v>9390</v>
+        <v>11980</v>
       </c>
       <c r="F45">
-        <v>9390</v>
+        <v>11980</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>12000</v>
       </c>
       <c r="C46">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
@@ -1867,13 +1861,13 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>12000</v>
       </c>
       <c r="C47">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
         <v>80</v>
@@ -1887,13 +1881,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>12000</v>
       </c>
       <c r="C48">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
         <v>80</v>
@@ -1907,22 +1901,22 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>12000</v>
       </c>
       <c r="C49">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E49">
-        <v>6260</v>
+        <v>9390</v>
       </c>
       <c r="F49">
-        <v>6260</v>
+        <v>9390</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1933,27 +1927,27 @@
         <v>12000</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50">
-        <v>11964</v>
+        <v>6260</v>
       </c>
       <c r="F50">
-        <v>11964</v>
+        <v>6260</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B51">
         <v>12000</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
         <v>82</v>
@@ -1967,13 +1961,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>12000</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
         <v>82</v>
@@ -1987,13 +1981,13 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <v>12000</v>
       </c>
       <c r="C53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53" t="s">
         <v>82</v>
@@ -2007,13 +2001,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54">
         <v>12000</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
         <v>82</v>
@@ -2027,13 +2021,13 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55">
         <v>12000</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
         <v>82</v>
@@ -2047,13 +2041,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56">
         <v>12000</v>
       </c>
       <c r="C56">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
         <v>82</v>
@@ -2067,13 +2061,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B57">
         <v>12000</v>
       </c>
       <c r="C57">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
         <v>82</v>
@@ -2087,13 +2081,13 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B58">
         <v>12000</v>
       </c>
       <c r="C58">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
         <v>82</v>
@@ -2107,42 +2101,42 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B59">
         <v>12000</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E59">
-        <v>11928</v>
+        <v>11964</v>
       </c>
       <c r="F59">
-        <v>11928</v>
+        <v>11964</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60">
         <v>12000</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E60">
-        <v>8946</v>
+        <v>11928</v>
       </c>
       <c r="F60">
-        <v>8946</v>
+        <v>11928</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2153,27 +2147,27 @@
         <v>12000</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E61">
-        <v>7958</v>
+        <v>8946</v>
       </c>
       <c r="F61">
-        <v>7958</v>
+        <v>8946</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B62">
         <v>12000</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
         <v>85</v>
@@ -2187,13 +2181,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B63">
         <v>12000</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
         <v>85</v>
@@ -2207,13 +2201,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B64">
         <v>12000</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
         <v>85</v>
@@ -2227,13 +2221,13 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B65">
         <v>12000</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D65" t="s">
         <v>85</v>
@@ -2247,13 +2241,13 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B66">
         <v>12000</v>
       </c>
       <c r="C66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D66" t="s">
         <v>85</v>
@@ -2267,62 +2261,62 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B67">
         <v>12000</v>
       </c>
       <c r="C67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E67">
-        <v>7953</v>
+        <v>7958</v>
       </c>
       <c r="F67">
-        <v>7953</v>
+        <v>7958</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>12000</v>
       </c>
       <c r="C68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E68">
-        <v>11978</v>
+        <v>7953</v>
       </c>
       <c r="F68">
-        <v>11978</v>
+        <v>7953</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <v>12000</v>
       </c>
       <c r="C69">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E69">
-        <v>2400</v>
+        <v>11978</v>
       </c>
       <c r="F69">
-        <v>2400</v>
+        <v>11978</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2333,27 +2327,27 @@
         <v>12000</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E70">
-        <v>11360</v>
+        <v>2400</v>
       </c>
       <c r="F70">
-        <v>11360</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B71">
         <v>12000</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" t="s">
         <v>89</v>
@@ -2367,13 +2361,13 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B72">
         <v>12000</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
         <v>89</v>
@@ -2387,13 +2381,13 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B73">
         <v>12000</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
         <v>89</v>
@@ -2407,62 +2401,62 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B74">
         <v>12000</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E74">
-        <v>11040</v>
+        <v>11360</v>
       </c>
       <c r="F74">
-        <v>11040</v>
+        <v>11360</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>12000</v>
       </c>
       <c r="C75">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E75">
-        <v>11680</v>
+        <v>11040</v>
       </c>
       <c r="F75">
-        <v>11680</v>
+        <v>11040</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B76">
         <v>12000</v>
       </c>
       <c r="C76">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E76">
-        <v>11200</v>
+        <v>11680</v>
       </c>
       <c r="F76">
-        <v>11200</v>
+        <v>11680</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2473,27 +2467,27 @@
         <v>12000</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E77">
-        <v>6329</v>
+        <v>11200</v>
       </c>
       <c r="F77">
-        <v>6329</v>
+        <v>11200</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B78">
         <v>12000</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" t="s">
         <v>93</v>
@@ -2507,13 +2501,13 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B79">
         <v>12000</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
         <v>93</v>
@@ -2527,13 +2521,13 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B80">
         <v>12000</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D80" t="s">
         <v>93</v>
@@ -2547,13 +2541,13 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B81">
         <v>12000</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D81" t="s">
         <v>93</v>
@@ -2567,93 +2561,93 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B82">
         <v>12000</v>
       </c>
       <c r="C82">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E82">
-        <v>10018</v>
+        <v>6329</v>
       </c>
       <c r="F82">
-        <v>10018</v>
+        <v>6329</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B83">
         <v>12000</v>
       </c>
       <c r="C83">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E83">
-        <v>11067</v>
+        <v>10018</v>
       </c>
       <c r="F83">
-        <v>11067</v>
+        <v>10018</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B84">
         <v>12000</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E84">
-        <v>10458</v>
+        <v>11067</v>
       </c>
       <c r="F84">
-        <v>10458</v>
+        <v>11067</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B85">
         <v>12000</v>
       </c>
       <c r="C85">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E85">
-        <v>9240</v>
+        <v>10458</v>
       </c>
       <c r="F85">
-        <v>9240</v>
+        <v>10458</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B86">
         <v>12000</v>
       </c>
       <c r="C86">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D86" t="s">
         <v>97</v>
@@ -2667,13 +2661,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B87">
         <v>12000</v>
       </c>
       <c r="C87">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
         <v>97</v>
@@ -2687,82 +2681,82 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B88">
         <v>12000</v>
       </c>
       <c r="C88">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E88">
-        <v>11557</v>
+        <v>9240</v>
       </c>
       <c r="F88">
-        <v>11557</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B89">
         <v>12000</v>
       </c>
       <c r="C89">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E89">
-        <v>10794</v>
+        <v>11557</v>
       </c>
       <c r="F89">
-        <v>10794</v>
+        <v>11557</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B90">
         <v>12000</v>
       </c>
       <c r="C90">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E90">
-        <v>11997</v>
+        <v>10794</v>
       </c>
       <c r="F90">
-        <v>11997</v>
+        <v>10794</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
+        <v>15</v>
+      </c>
+      <c r="B91">
+        <v>12000</v>
+      </c>
+      <c r="C91">
         <v>14</v>
       </c>
-      <c r="B91">
-        <v>12000</v>
-      </c>
-      <c r="C91">
-        <v>15</v>
-      </c>
       <c r="D91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E91">
-        <v>4768</v>
+        <v>11997</v>
       </c>
       <c r="F91">
-        <v>4768</v>
+        <v>11997</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2773,36 +2767,36 @@
         <v>12000</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E92">
-        <v>11844</v>
+        <v>4768</v>
       </c>
       <c r="F92">
-        <v>11844</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B93">
         <v>12000</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E93">
-        <v>6956</v>
+        <v>11844</v>
       </c>
       <c r="F93">
-        <v>6956</v>
+        <v>11844</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2813,16 +2807,16 @@
         <v>12000</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E94">
-        <v>8624</v>
+        <v>6956</v>
       </c>
       <c r="F94">
-        <v>8624</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2836,13 +2830,13 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E95">
-        <v>2720</v>
+        <v>8624</v>
       </c>
       <c r="F95">
-        <v>2720</v>
+        <v>8624</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2856,13 +2850,13 @@
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E96">
-        <v>1916</v>
+        <v>2720</v>
       </c>
       <c r="F96">
-        <v>1916</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2876,13 +2870,13 @@
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E97">
-        <v>314</v>
+        <v>1916</v>
       </c>
       <c r="F97">
-        <v>314</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2896,13 +2890,13 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E98">
-        <v>3926</v>
+        <v>314</v>
       </c>
       <c r="F98">
-        <v>3926</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2916,13 +2910,13 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E99">
-        <v>1224</v>
+        <v>3926</v>
       </c>
       <c r="F99">
-        <v>1224</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2936,13 +2930,13 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E100">
-        <v>408</v>
+        <v>1224</v>
       </c>
       <c r="F100">
-        <v>408</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2956,13 +2950,13 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E101">
-        <v>1356</v>
+        <v>408</v>
       </c>
       <c r="F101">
-        <v>1356</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2976,13 +2970,13 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E102">
-        <v>452</v>
+        <v>1356</v>
       </c>
       <c r="F102">
-        <v>452</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2996,13 +2990,13 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E103">
-        <v>904</v>
+        <v>452</v>
       </c>
       <c r="F103">
-        <v>904</v>
+        <v>452</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3016,13 +3010,13 @@
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E104">
-        <v>1500</v>
+        <v>904</v>
       </c>
       <c r="F104">
-        <v>1500</v>
+        <v>904</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3036,13 +3030,13 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E105">
-        <v>744</v>
+        <v>1500</v>
       </c>
       <c r="F105">
-        <v>744</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3056,13 +3050,13 @@
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E106">
-        <v>786</v>
+        <v>744</v>
       </c>
       <c r="F106">
-        <v>786</v>
+        <v>744</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3076,13 +3070,13 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E107">
-        <v>220</v>
+        <v>786</v>
       </c>
       <c r="F107">
-        <v>220</v>
+        <v>786</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3096,33 +3090,33 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E108">
-        <v>11968</v>
+        <v>220</v>
       </c>
       <c r="F108">
-        <v>11968</v>
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B109">
         <v>12000</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E109">
-        <v>3984</v>
+        <v>11968</v>
       </c>
       <c r="F109">
-        <v>3984</v>
+        <v>11968</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3133,36 +3127,36 @@
         <v>12000</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E110">
-        <v>11725</v>
+        <v>3984</v>
       </c>
       <c r="F110">
-        <v>11725</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B111">
         <v>12000</v>
       </c>
       <c r="C111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E111">
-        <v>4355</v>
+        <v>11725</v>
       </c>
       <c r="F111">
-        <v>4355</v>
+        <v>11725</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3173,16 +3167,16 @@
         <v>12000</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D112" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E112">
-        <v>3960</v>
+        <v>4355</v>
       </c>
       <c r="F112">
-        <v>3960</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3196,13 +3190,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E113">
-        <v>240</v>
+        <v>3960</v>
       </c>
       <c r="F113">
-        <v>240</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3216,13 +3210,13 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E114">
-        <v>2384</v>
+        <v>240</v>
       </c>
       <c r="F114">
-        <v>2384</v>
+        <v>240</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3236,33 +3230,33 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E115">
-        <v>11956</v>
+        <v>2384</v>
       </c>
       <c r="F115">
-        <v>11956</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B116">
         <v>12000</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E116">
-        <v>11468</v>
+        <v>11956</v>
       </c>
       <c r="F116">
-        <v>11468</v>
+        <v>11956</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3273,16 +3267,16 @@
         <v>12000</v>
       </c>
       <c r="C117">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E117">
-        <v>308</v>
+        <v>11468</v>
       </c>
       <c r="F117">
-        <v>308</v>
+        <v>11468</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3296,13 +3290,13 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E118">
-        <v>1816</v>
+        <v>308</v>
       </c>
       <c r="F118">
-        <v>1816</v>
+        <v>308</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3316,13 +3310,13 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E119">
-        <v>734</v>
+        <v>1816</v>
       </c>
       <c r="F119">
-        <v>734</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3336,13 +3330,13 @@
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E120">
-        <v>1572</v>
+        <v>734</v>
       </c>
       <c r="F120">
-        <v>1572</v>
+        <v>734</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3356,13 +3350,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E121">
-        <v>2451</v>
+        <v>1572</v>
       </c>
       <c r="F121">
-        <v>2451</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3376,13 +3370,13 @@
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E122">
-        <v>515</v>
+        <v>2451</v>
       </c>
       <c r="F122">
-        <v>515</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3396,13 +3390,13 @@
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E123">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F123">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3416,13 +3410,13 @@
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E124">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="F124">
-        <v>515</v>
+        <v>521</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3436,13 +3430,13 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="E125">
-        <v>1916</v>
+        <v>515</v>
       </c>
       <c r="F125">
-        <v>1916</v>
+        <v>515</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3456,13 +3450,13 @@
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="E126">
-        <v>1812</v>
+        <v>1916</v>
       </c>
       <c r="F126">
-        <v>1812</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3476,13 +3470,13 @@
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E127">
-        <v>2548</v>
+        <v>1812</v>
       </c>
       <c r="F127">
-        <v>2548</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3496,13 +3490,13 @@
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E128">
-        <v>1248</v>
+        <v>2548</v>
       </c>
       <c r="F128">
-        <v>1248</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3516,13 +3510,13 @@
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E129">
-        <v>649</v>
+        <v>1248</v>
       </c>
       <c r="F129">
-        <v>649</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3536,13 +3530,13 @@
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E130">
-        <v>1540</v>
+        <v>649</v>
       </c>
       <c r="F130">
-        <v>1540</v>
+        <v>649</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3556,13 +3550,13 @@
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E131">
-        <v>650</v>
+        <v>1540</v>
       </c>
       <c r="F131">
-        <v>650</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3576,13 +3570,13 @@
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E132">
-        <v>1256</v>
+        <v>650</v>
       </c>
       <c r="F132">
-        <v>1256</v>
+        <v>650</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3596,13 +3590,13 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E133">
-        <v>1448</v>
+        <v>1256</v>
       </c>
       <c r="F133">
-        <v>1448</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3616,13 +3610,13 @@
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="E134">
-        <v>3926</v>
+        <v>1448</v>
       </c>
       <c r="F134">
-        <v>3926</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3636,33 +3630,33 @@
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="E135">
-        <v>12000</v>
+        <v>3926</v>
       </c>
       <c r="F135">
-        <v>12000</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B136">
         <v>12000</v>
       </c>
       <c r="C136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E136">
-        <v>800</v>
+        <v>12000</v>
       </c>
       <c r="F136">
-        <v>800</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3673,16 +3667,16 @@
         <v>12000</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E137">
-        <v>2760</v>
+        <v>800</v>
       </c>
       <c r="F137">
-        <v>2760</v>
+        <v>800</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3696,13 +3690,13 @@
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E138">
-        <v>3200</v>
+        <v>2760</v>
       </c>
       <c r="F138">
-        <v>3200</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3716,33 +3710,33 @@
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E139">
-        <v>12000</v>
+        <v>3200</v>
       </c>
       <c r="F139">
-        <v>12000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B140">
         <v>12000</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D140" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E140">
-        <v>9680</v>
+        <v>12000</v>
       </c>
       <c r="F140">
-        <v>9680</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3753,16 +3747,16 @@
         <v>12000</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E141">
-        <v>4000</v>
+        <v>9680</v>
       </c>
       <c r="F141">
-        <v>4000</v>
+        <v>9680</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3776,13 +3770,13 @@
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E142">
-        <v>1100</v>
+        <v>4000</v>
       </c>
       <c r="F142">
-        <v>1100</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -3796,13 +3790,13 @@
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E143">
-        <v>920</v>
+        <v>1100</v>
       </c>
       <c r="F143">
-        <v>920</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -3816,13 +3810,13 @@
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E144">
-        <v>3200</v>
+        <v>920</v>
       </c>
       <c r="F144">
-        <v>3200</v>
+        <v>920</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -3836,33 +3830,33 @@
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E145">
-        <v>11400</v>
+        <v>3200</v>
       </c>
       <c r="F145">
-        <v>11400</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B146">
         <v>12000</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E146">
-        <v>3780</v>
+        <v>11400</v>
       </c>
       <c r="F146">
-        <v>3780</v>
+        <v>11400</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -3873,16 +3867,16 @@
         <v>12000</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E147">
-        <v>8000</v>
+        <v>3780</v>
       </c>
       <c r="F147">
-        <v>8000</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -3896,13 +3890,13 @@
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E148">
-        <v>326</v>
+        <v>8000</v>
       </c>
       <c r="F148">
-        <v>326</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -3916,13 +3910,13 @@
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E149">
-        <v>780</v>
+        <v>326</v>
       </c>
       <c r="F149">
-        <v>780</v>
+        <v>326</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -3936,13 +3930,13 @@
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E150">
-        <v>5779</v>
+        <v>780</v>
       </c>
       <c r="F150">
-        <v>5779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -3956,24 +3950,24 @@
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E151">
-        <v>6152</v>
+        <v>5779</v>
       </c>
       <c r="F151">
-        <v>6152</v>
+        <v>5779</v>
       </c>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B152">
         <v>12000</v>
       </c>
       <c r="C152">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D152" t="s">
         <v>158</v>
@@ -3987,13 +3981,13 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B153">
         <v>12000</v>
       </c>
       <c r="C153">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D153" t="s">
         <v>158</v>
@@ -4007,13 +4001,13 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B154">
         <v>12000</v>
       </c>
       <c r="C154">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D154" t="s">
         <v>158</v>
@@ -4027,33 +4021,33 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B155">
         <v>12000</v>
       </c>
       <c r="C155">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D155" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E155">
-        <v>11730</v>
+        <v>6152</v>
       </c>
       <c r="F155">
-        <v>11730</v>
+        <v>6152</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B156">
         <v>12000</v>
       </c>
       <c r="C156">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D156" t="s">
         <v>159</v>
@@ -4067,202 +4061,202 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B157">
         <v>12000</v>
       </c>
       <c r="C157">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D157" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E157">
-        <v>11427</v>
+        <v>11730</v>
       </c>
       <c r="F157">
-        <v>11427</v>
+        <v>11730</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B158">
         <v>12000</v>
       </c>
       <c r="C158">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D158" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E158">
-        <v>11139</v>
+        <v>11427</v>
       </c>
       <c r="F158">
-        <v>11139</v>
+        <v>11427</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B159">
         <v>12000</v>
       </c>
       <c r="C159">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D159" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E159">
-        <v>10343</v>
+        <v>11139</v>
       </c>
       <c r="F159">
-        <v>10343</v>
+        <v>11139</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B160">
         <v>12000</v>
       </c>
       <c r="C160">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E160">
-        <v>11919</v>
+        <v>10343</v>
       </c>
       <c r="F160">
-        <v>11919</v>
+        <v>10343</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B161">
         <v>12000</v>
       </c>
       <c r="C161">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E161">
-        <v>11442</v>
+        <v>11919</v>
       </c>
       <c r="F161">
-        <v>11442</v>
+        <v>11919</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B162">
         <v>12000</v>
       </c>
       <c r="C162">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D162" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E162">
-        <v>11185</v>
+        <v>11442</v>
       </c>
       <c r="F162">
-        <v>11185</v>
+        <v>11442</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B163">
         <v>12000</v>
       </c>
       <c r="C163">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E163">
-        <v>10410</v>
+        <v>11185</v>
       </c>
       <c r="F163">
-        <v>10410</v>
+        <v>11185</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B164">
         <v>12000</v>
       </c>
       <c r="C164">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E164">
-        <v>10998</v>
+        <v>10410</v>
       </c>
       <c r="F164">
-        <v>10998</v>
+        <v>10410</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B165">
         <v>12000</v>
       </c>
       <c r="C165">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D165" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E165">
-        <v>10617</v>
+        <v>10998</v>
       </c>
       <c r="F165">
-        <v>10617</v>
+        <v>10998</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B166">
         <v>12000</v>
       </c>
       <c r="C166">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D166" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E166">
-        <v>5253</v>
+        <v>10617</v>
       </c>
       <c r="F166">
-        <v>5253</v>
+        <v>10617</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -4273,56 +4267,56 @@
         <v>12000</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E167">
-        <v>10314</v>
+        <v>5253</v>
       </c>
       <c r="F167">
-        <v>10314</v>
+        <v>5253</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B168">
         <v>12000</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E168">
-        <v>11723</v>
+        <v>10314</v>
       </c>
       <c r="F168">
-        <v>11723</v>
+        <v>10314</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B169">
         <v>12000</v>
       </c>
       <c r="C169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E169">
-        <v>4800</v>
+        <v>11723</v>
       </c>
       <c r="F169">
-        <v>4800</v>
+        <v>11723</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -4333,36 +4327,16 @@
         <v>12000</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E170">
-        <v>4500</v>
+        <v>4800</v>
       </c>
       <c r="F170">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="A171" t="s">
-        <v>70</v>
-      </c>
-      <c r="B171">
-        <v>12000</v>
-      </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-      <c r="D171" t="s">
-        <v>174</v>
-      </c>
-      <c r="E171">
-        <v>4500</v>
-      </c>
-      <c r="F171">
-        <v>4500</v>
+        <v>4800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance Cutting Optimizer Pro functionality and user interface: - Updated .gitignore to include new Excel files and temporary locks. - Improved data loading and cleaning in co.py with enhanced debugging and error handling. - Added weight calculation features and statistics in the optimization process. - Updated GUI in gui.py to include new settings for weight error margin and steel price. - Enhanced translations.json with new keys for weight-related results. - Updated optimized_cutting_plan.xlsx and cutting_plan.png to reflect changes in calculations and outputs.
</commit_message>
<xml_diff>
--- a/optimized_cutting_plan.xlsx
+++ b/optimized_cutting_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="171">
   <si>
     <t>Profile</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Remaining Length</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>HEA140</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
   </si>
   <si>
     <t>UPN200</t>
-  </si>
-  <si>
-    <t>[0, 0, 0, 0]</t>
   </si>
   <si>
     <t>[1435, 1435]</t>
@@ -617,8 +611,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>18</xdr:colOff>
-      <xdr:row>615</xdr:row>
-      <xdr:rowOff>76434</xdr:rowOff>
+      <xdr:row>605</xdr:row>
+      <xdr:rowOff>152630</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -636,7 +630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4267200" y="190500"/>
-          <a:ext cx="9144018" cy="117043434"/>
+          <a:ext cx="9144018" cy="115214630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -933,7 +927,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -970,13 +964,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2870</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -990,47 +984,47 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3">
-        <v>2870</v>
+        <v>11962</v>
       </c>
       <c r="F3">
-        <v>2870</v>
+        <v>11962</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>12000</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4">
-        <v>11962</v>
+        <v>11924</v>
       </c>
       <c r="F4">
-        <v>11962</v>
+        <v>11924</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>12000</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5">
         <v>11924</v>
@@ -1041,22 +1035,22 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>12000</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6">
-        <v>11924</v>
+        <v>8886</v>
       </c>
       <c r="F6">
-        <v>11924</v>
+        <v>8886</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1067,30 +1061,30 @@
         <v>12000</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E7">
-        <v>8886</v>
+        <v>11924</v>
       </c>
       <c r="F7">
-        <v>8886</v>
+        <v>11924</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>12000</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8">
         <v>11924</v>
@@ -1101,16 +1095,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>12000</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9">
         <v>11924</v>
@@ -1121,16 +1115,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>12000</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>11924</v>
@@ -1141,22 +1135,22 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>12000</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>73</v>
       </c>
       <c r="E11">
-        <v>11924</v>
+        <v>11848</v>
       </c>
       <c r="F11">
-        <v>11924</v>
+        <v>11848</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1167,30 +1161,30 @@
         <v>12000</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12">
-        <v>11848</v>
+        <v>6579</v>
       </c>
       <c r="F12">
-        <v>11848</v>
+        <v>6579</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>12000</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13">
         <v>6579</v>
@@ -1201,16 +1195,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>12000</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14">
         <v>6579</v>
@@ -1221,16 +1215,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>12000</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>6579</v>
@@ -1241,16 +1235,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>12000</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E16">
         <v>6579</v>
@@ -1261,16 +1255,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>12000</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E17">
         <v>6579</v>
@@ -1281,16 +1275,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>12000</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18">
         <v>6579</v>
@@ -1301,16 +1295,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>12000</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19">
         <v>6579</v>
@@ -1321,36 +1315,36 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>12000</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20">
-        <v>6579</v>
+        <v>11940</v>
       </c>
       <c r="F20">
-        <v>6579</v>
+        <v>11940</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>12000</v>
+      </c>
+      <c r="C21">
         <v>10</v>
       </c>
-      <c r="B21">
-        <v>12000</v>
-      </c>
-      <c r="C21">
-        <v>9</v>
-      </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <v>11940</v>
@@ -1361,16 +1355,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>12000</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22">
         <v>11940</v>
@@ -1381,16 +1375,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>12000</v>
       </c>
       <c r="C23">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>11940</v>
@@ -1407,30 +1401,30 @@
         <v>12000</v>
       </c>
       <c r="C24">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24">
-        <v>11940</v>
+        <v>6130</v>
       </c>
       <c r="F24">
-        <v>11940</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>12000</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>6130</v>
@@ -1441,16 +1435,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>12000</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E26">
         <v>6130</v>
@@ -1461,16 +1455,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>12000</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E27">
         <v>6130</v>
@@ -1481,16 +1475,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>12000</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>6130</v>
@@ -1501,16 +1495,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>12000</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>6130</v>
@@ -1521,16 +1515,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>12000</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>6130</v>
@@ -1541,16 +1535,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>12000</v>
       </c>
       <c r="C31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>6130</v>
@@ -1561,16 +1555,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>12000</v>
       </c>
       <c r="C32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E32">
         <v>6130</v>
@@ -1581,16 +1575,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>12000</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E33">
         <v>6130</v>
@@ -1601,16 +1595,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>12000</v>
+      </c>
+      <c r="C34">
         <v>11</v>
       </c>
-      <c r="B34">
-        <v>12000</v>
-      </c>
-      <c r="C34">
-        <v>10</v>
-      </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E34">
         <v>6130</v>
@@ -1621,16 +1615,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35">
         <v>12000</v>
       </c>
       <c r="C35">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>6130</v>
@@ -1641,16 +1635,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>12000</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <v>6130</v>
@@ -1661,16 +1655,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>12000</v>
       </c>
       <c r="C37">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37">
         <v>6130</v>
@@ -1681,36 +1675,36 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>12000</v>
       </c>
       <c r="C38">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E38">
-        <v>6130</v>
+        <v>11980</v>
       </c>
       <c r="F38">
-        <v>6130</v>
+        <v>11980</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>12000</v>
       </c>
       <c r="C39">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E39">
         <v>11980</v>
@@ -1721,16 +1715,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>12000</v>
       </c>
       <c r="C40">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E40">
         <v>11980</v>
@@ -1741,16 +1735,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>12000</v>
       </c>
       <c r="C41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E41">
         <v>11980</v>
@@ -1761,16 +1755,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>12000</v>
       </c>
       <c r="C42">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E42">
         <v>11980</v>
@@ -1781,16 +1775,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>12000</v>
       </c>
       <c r="C43">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E43">
         <v>11980</v>
@@ -1801,16 +1795,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
         <v>12000</v>
       </c>
       <c r="C44">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E44">
         <v>11980</v>
@@ -1821,36 +1815,36 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>12000</v>
       </c>
       <c r="C45">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E45">
-        <v>11980</v>
+        <v>9390</v>
       </c>
       <c r="F45">
-        <v>11980</v>
+        <v>9390</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46">
         <v>12000</v>
       </c>
       <c r="C46">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E46">
         <v>9390</v>
@@ -1861,16 +1855,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47">
         <v>12000</v>
       </c>
       <c r="C47">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E47">
         <v>9390</v>
@@ -1881,16 +1875,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48">
         <v>12000</v>
       </c>
       <c r="C48">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E48">
         <v>9390</v>
@@ -1901,22 +1895,22 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49">
         <v>12000</v>
       </c>
       <c r="C49">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E49">
-        <v>9390</v>
+        <v>6260</v>
       </c>
       <c r="F49">
-        <v>9390</v>
+        <v>6260</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1927,30 +1921,30 @@
         <v>12000</v>
       </c>
       <c r="C50">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E50">
-        <v>6260</v>
+        <v>11964</v>
       </c>
       <c r="F50">
-        <v>6260</v>
+        <v>11964</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51">
         <v>12000</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E51">
         <v>11964</v>
@@ -1961,16 +1955,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B52">
         <v>12000</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E52">
         <v>11964</v>
@@ -1981,16 +1975,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53">
         <v>12000</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E53">
         <v>11964</v>
@@ -2001,16 +1995,16 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54">
         <v>12000</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E54">
         <v>11964</v>
@@ -2021,16 +2015,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55">
         <v>12000</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E55">
         <v>11964</v>
@@ -2041,16 +2035,16 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56">
         <v>12000</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E56">
         <v>11964</v>
@@ -2061,16 +2055,16 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B57">
         <v>12000</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E57">
         <v>11964</v>
@@ -2081,16 +2075,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B58">
         <v>12000</v>
       </c>
       <c r="C58">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E58">
         <v>11964</v>
@@ -2101,42 +2095,42 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59">
         <v>12000</v>
       </c>
       <c r="C59">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59">
-        <v>11964</v>
+        <v>11928</v>
       </c>
       <c r="F59">
-        <v>11964</v>
+        <v>11928</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B60">
         <v>12000</v>
       </c>
       <c r="C60">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60">
-        <v>11928</v>
+        <v>8946</v>
       </c>
       <c r="F60">
-        <v>11928</v>
+        <v>8946</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2147,30 +2141,30 @@
         <v>12000</v>
       </c>
       <c r="C61">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E61">
-        <v>8946</v>
+        <v>7958</v>
       </c>
       <c r="F61">
-        <v>8946</v>
+        <v>7958</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62">
         <v>12000</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E62">
         <v>7958</v>
@@ -2181,16 +2175,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B63">
         <v>12000</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E63">
         <v>7958</v>
@@ -2201,16 +2195,16 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B64">
         <v>12000</v>
       </c>
       <c r="C64">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E64">
         <v>7958</v>
@@ -2221,16 +2215,16 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B65">
         <v>12000</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E65">
         <v>7958</v>
@@ -2241,16 +2235,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66">
         <v>12000</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E66">
         <v>7958</v>
@@ -2261,62 +2255,62 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>12000</v>
       </c>
       <c r="C67">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E67">
-        <v>7958</v>
+        <v>7953</v>
       </c>
       <c r="F67">
-        <v>7958</v>
+        <v>7953</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B68">
         <v>12000</v>
       </c>
       <c r="C68">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E68">
-        <v>7953</v>
+        <v>11978</v>
       </c>
       <c r="F68">
-        <v>7953</v>
+        <v>11978</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B69">
         <v>12000</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E69">
-        <v>11978</v>
+        <v>2400</v>
       </c>
       <c r="F69">
-        <v>11978</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2327,30 +2321,30 @@
         <v>12000</v>
       </c>
       <c r="C70">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E70">
-        <v>2400</v>
+        <v>11360</v>
       </c>
       <c r="F70">
-        <v>2400</v>
+        <v>11360</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B71">
         <v>12000</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E71">
         <v>11360</v>
@@ -2361,16 +2355,16 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72">
         <v>12000</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E72">
         <v>11360</v>
@@ -2381,16 +2375,16 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73">
         <v>12000</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D73" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E73">
         <v>11360</v>
@@ -2401,62 +2395,62 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B74">
         <v>12000</v>
       </c>
       <c r="C74">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E74">
-        <v>11360</v>
+        <v>11040</v>
       </c>
       <c r="F74">
-        <v>11360</v>
+        <v>11040</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B75">
         <v>12000</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E75">
-        <v>11040</v>
+        <v>11680</v>
       </c>
       <c r="F75">
-        <v>11040</v>
+        <v>11680</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76">
         <v>12000</v>
       </c>
       <c r="C76">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E76">
-        <v>11680</v>
+        <v>11200</v>
       </c>
       <c r="F76">
-        <v>11680</v>
+        <v>11200</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2467,30 +2461,30 @@
         <v>12000</v>
       </c>
       <c r="C77">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E77">
-        <v>11200</v>
+        <v>6329</v>
       </c>
       <c r="F77">
-        <v>11200</v>
+        <v>6329</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B78">
         <v>12000</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E78">
         <v>6329</v>
@@ -2501,16 +2495,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B79">
         <v>12000</v>
       </c>
       <c r="C79">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E79">
         <v>6329</v>
@@ -2521,16 +2515,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B80">
         <v>12000</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E80">
         <v>6329</v>
@@ -2541,16 +2535,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B81">
         <v>12000</v>
       </c>
       <c r="C81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E81">
         <v>6329</v>
@@ -2561,96 +2555,96 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B82">
         <v>12000</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E82">
-        <v>6329</v>
+        <v>10018</v>
       </c>
       <c r="F82">
-        <v>6329</v>
+        <v>10018</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B83">
         <v>12000</v>
       </c>
       <c r="C83">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E83">
-        <v>10018</v>
+        <v>11067</v>
       </c>
       <c r="F83">
-        <v>10018</v>
+        <v>11067</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>12000</v>
       </c>
       <c r="C84">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E84">
-        <v>11067</v>
+        <v>10458</v>
       </c>
       <c r="F84">
-        <v>11067</v>
+        <v>10458</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B85">
         <v>12000</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E85">
-        <v>10458</v>
+        <v>9240</v>
       </c>
       <c r="F85">
-        <v>10458</v>
+        <v>9240</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B86">
         <v>12000</v>
       </c>
       <c r="C86">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E86">
         <v>9240</v>
@@ -2661,16 +2655,16 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B87">
         <v>12000</v>
       </c>
       <c r="C87">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E87">
         <v>9240</v>
@@ -2681,82 +2675,82 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B88">
         <v>12000</v>
       </c>
       <c r="C88">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E88">
-        <v>9240</v>
+        <v>11557</v>
       </c>
       <c r="F88">
-        <v>9240</v>
+        <v>11557</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B89">
         <v>12000</v>
       </c>
       <c r="C89">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E89">
-        <v>11557</v>
+        <v>10794</v>
       </c>
       <c r="F89">
-        <v>11557</v>
+        <v>10794</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B90">
         <v>12000</v>
       </c>
       <c r="C90">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E90">
-        <v>10794</v>
+        <v>11997</v>
       </c>
       <c r="F90">
-        <v>10794</v>
+        <v>11997</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91">
+        <v>12000</v>
+      </c>
+      <c r="C91">
         <v>15</v>
       </c>
-      <c r="B91">
-        <v>12000</v>
-      </c>
-      <c r="C91">
-        <v>14</v>
-      </c>
       <c r="D91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E91">
-        <v>11997</v>
+        <v>4768</v>
       </c>
       <c r="F91">
-        <v>11997</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2767,36 +2761,36 @@
         <v>12000</v>
       </c>
       <c r="C92">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E92">
-        <v>4768</v>
+        <v>11844</v>
       </c>
       <c r="F92">
-        <v>4768</v>
+        <v>11844</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B93">
         <v>12000</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E93">
-        <v>11844</v>
+        <v>6956</v>
       </c>
       <c r="F93">
-        <v>11844</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2807,16 +2801,16 @@
         <v>12000</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E94">
-        <v>6956</v>
+        <v>8624</v>
       </c>
       <c r="F94">
-        <v>6956</v>
+        <v>8624</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2830,13 +2824,13 @@
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E95">
-        <v>8624</v>
+        <v>2720</v>
       </c>
       <c r="F95">
-        <v>8624</v>
+        <v>2720</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2850,13 +2844,13 @@
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E96">
-        <v>2720</v>
+        <v>1916</v>
       </c>
       <c r="F96">
-        <v>2720</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2870,13 +2864,13 @@
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97">
-        <v>1916</v>
+        <v>314</v>
       </c>
       <c r="F97">
-        <v>1916</v>
+        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2890,13 +2884,13 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98">
-        <v>314</v>
+        <v>3926</v>
       </c>
       <c r="F98">
-        <v>314</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2910,13 +2904,13 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E99">
-        <v>3926</v>
+        <v>1224</v>
       </c>
       <c r="F99">
-        <v>3926</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2930,13 +2924,13 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E100">
-        <v>1224</v>
+        <v>408</v>
       </c>
       <c r="F100">
-        <v>1224</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2950,13 +2944,13 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E101">
-        <v>408</v>
+        <v>1356</v>
       </c>
       <c r="F101">
-        <v>408</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2970,13 +2964,13 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E102">
-        <v>1356</v>
+        <v>452</v>
       </c>
       <c r="F102">
-        <v>1356</v>
+        <v>452</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2990,13 +2984,13 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E103">
-        <v>452</v>
+        <v>904</v>
       </c>
       <c r="F103">
-        <v>452</v>
+        <v>904</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3010,13 +3004,13 @@
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E104">
-        <v>904</v>
+        <v>1500</v>
       </c>
       <c r="F104">
-        <v>904</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3030,13 +3024,13 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E105">
-        <v>1500</v>
+        <v>744</v>
       </c>
       <c r="F105">
-        <v>1500</v>
+        <v>744</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3050,13 +3044,13 @@
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E106">
-        <v>744</v>
+        <v>786</v>
       </c>
       <c r="F106">
-        <v>744</v>
+        <v>786</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3070,13 +3064,13 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E107">
-        <v>786</v>
+        <v>220</v>
       </c>
       <c r="F107">
-        <v>786</v>
+        <v>220</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3090,33 +3084,33 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E108">
-        <v>220</v>
+        <v>11968</v>
       </c>
       <c r="F108">
-        <v>220</v>
+        <v>11968</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B109">
         <v>12000</v>
       </c>
       <c r="C109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E109">
-        <v>11968</v>
+        <v>3984</v>
       </c>
       <c r="F109">
-        <v>11968</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -3127,36 +3121,36 @@
         <v>12000</v>
       </c>
       <c r="C110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D110" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E110">
-        <v>3984</v>
+        <v>11725</v>
       </c>
       <c r="F110">
-        <v>3984</v>
+        <v>11725</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B111">
         <v>12000</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E111">
-        <v>11725</v>
+        <v>4355</v>
       </c>
       <c r="F111">
-        <v>11725</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3167,16 +3161,16 @@
         <v>12000</v>
       </c>
       <c r="C112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E112">
-        <v>4355</v>
+        <v>3960</v>
       </c>
       <c r="F112">
-        <v>4355</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3190,13 +3184,13 @@
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E113">
-        <v>3960</v>
+        <v>240</v>
       </c>
       <c r="F113">
-        <v>3960</v>
+        <v>240</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3210,13 +3204,13 @@
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E114">
-        <v>240</v>
+        <v>2384</v>
       </c>
       <c r="F114">
-        <v>240</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3230,33 +3224,33 @@
         <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E115">
-        <v>2384</v>
+        <v>11956</v>
       </c>
       <c r="F115">
-        <v>2384</v>
+        <v>11956</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B116">
         <v>12000</v>
       </c>
       <c r="C116">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E116">
-        <v>11956</v>
+        <v>11468</v>
       </c>
       <c r="F116">
-        <v>11956</v>
+        <v>11468</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3267,16 +3261,16 @@
         <v>12000</v>
       </c>
       <c r="C117">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E117">
-        <v>11468</v>
+        <v>308</v>
       </c>
       <c r="F117">
-        <v>11468</v>
+        <v>308</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3290,13 +3284,13 @@
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E118">
-        <v>308</v>
+        <v>1816</v>
       </c>
       <c r="F118">
-        <v>308</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3310,13 +3304,13 @@
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E119">
-        <v>1816</v>
+        <v>734</v>
       </c>
       <c r="F119">
-        <v>1816</v>
+        <v>734</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3330,13 +3324,13 @@
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E120">
-        <v>734</v>
+        <v>1572</v>
       </c>
       <c r="F120">
-        <v>734</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3350,13 +3344,13 @@
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E121">
-        <v>1572</v>
+        <v>2451</v>
       </c>
       <c r="F121">
-        <v>1572</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3370,13 +3364,13 @@
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E122">
-        <v>2451</v>
+        <v>515</v>
       </c>
       <c r="F122">
-        <v>2451</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3390,13 +3384,13 @@
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E123">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="F123">
-        <v>515</v>
+        <v>521</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3410,13 +3404,13 @@
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E124">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F124">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3430,13 +3424,13 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="E125">
-        <v>515</v>
+        <v>1916</v>
       </c>
       <c r="F125">
-        <v>515</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3450,13 +3444,13 @@
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="E126">
-        <v>1916</v>
+        <v>1812</v>
       </c>
       <c r="F126">
-        <v>1916</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3470,13 +3464,13 @@
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E127">
-        <v>1812</v>
+        <v>2548</v>
       </c>
       <c r="F127">
-        <v>1812</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3490,13 +3484,13 @@
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E128">
-        <v>2548</v>
+        <v>1248</v>
       </c>
       <c r="F128">
-        <v>2548</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3510,13 +3504,13 @@
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E129">
-        <v>1248</v>
+        <v>649</v>
       </c>
       <c r="F129">
-        <v>1248</v>
+        <v>649</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3530,13 +3524,13 @@
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E130">
-        <v>649</v>
+        <v>1540</v>
       </c>
       <c r="F130">
-        <v>649</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3550,13 +3544,13 @@
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E131">
-        <v>1540</v>
+        <v>650</v>
       </c>
       <c r="F131">
-        <v>1540</v>
+        <v>650</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3570,13 +3564,13 @@
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E132">
-        <v>650</v>
+        <v>1256</v>
       </c>
       <c r="F132">
-        <v>650</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3590,13 +3584,13 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E133">
-        <v>1256</v>
+        <v>1448</v>
       </c>
       <c r="F133">
-        <v>1256</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3610,13 +3604,13 @@
         <v>1</v>
       </c>
       <c r="D134" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="E134">
-        <v>1448</v>
+        <v>3926</v>
       </c>
       <c r="F134">
-        <v>1448</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3630,33 +3624,33 @@
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="E135">
-        <v>3926</v>
+        <v>12000</v>
       </c>
       <c r="F135">
-        <v>3926</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B136">
         <v>12000</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E136">
-        <v>12000</v>
+        <v>800</v>
       </c>
       <c r="F136">
-        <v>12000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3667,16 +3661,16 @@
         <v>12000</v>
       </c>
       <c r="C137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E137">
-        <v>800</v>
+        <v>2760</v>
       </c>
       <c r="F137">
-        <v>800</v>
+        <v>2760</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3690,13 +3684,13 @@
         <v>1</v>
       </c>
       <c r="D138" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E138">
-        <v>2760</v>
+        <v>3200</v>
       </c>
       <c r="F138">
-        <v>2760</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3710,33 +3704,33 @@
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E139">
-        <v>3200</v>
+        <v>12000</v>
       </c>
       <c r="F139">
-        <v>3200</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B140">
         <v>12000</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E140">
-        <v>12000</v>
+        <v>9680</v>
       </c>
       <c r="F140">
-        <v>12000</v>
+        <v>9680</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3747,16 +3741,16 @@
         <v>12000</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E141">
-        <v>9680</v>
+        <v>4000</v>
       </c>
       <c r="F141">
-        <v>9680</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -3770,13 +3764,13 @@
         <v>1</v>
       </c>
       <c r="D142" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E142">
-        <v>4000</v>
+        <v>1100</v>
       </c>
       <c r="F142">
-        <v>4000</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -3790,13 +3784,13 @@
         <v>1</v>
       </c>
       <c r="D143" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E143">
-        <v>1100</v>
+        <v>920</v>
       </c>
       <c r="F143">
-        <v>1100</v>
+        <v>920</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -3810,13 +3804,13 @@
         <v>1</v>
       </c>
       <c r="D144" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E144">
-        <v>920</v>
+        <v>3200</v>
       </c>
       <c r="F144">
-        <v>920</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -3830,33 +3824,33 @@
         <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E145">
-        <v>3200</v>
+        <v>11400</v>
       </c>
       <c r="F145">
-        <v>3200</v>
+        <v>11400</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B146">
         <v>12000</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E146">
-        <v>11400</v>
+        <v>3780</v>
       </c>
       <c r="F146">
-        <v>11400</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -3867,16 +3861,16 @@
         <v>12000</v>
       </c>
       <c r="C147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E147">
-        <v>3780</v>
+        <v>8000</v>
       </c>
       <c r="F147">
-        <v>3780</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -3890,13 +3884,13 @@
         <v>1</v>
       </c>
       <c r="D148" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E148">
-        <v>8000</v>
+        <v>326</v>
       </c>
       <c r="F148">
-        <v>8000</v>
+        <v>326</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -3910,13 +3904,13 @@
         <v>1</v>
       </c>
       <c r="D149" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E149">
-        <v>326</v>
+        <v>780</v>
       </c>
       <c r="F149">
-        <v>326</v>
+        <v>780</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -3930,13 +3924,13 @@
         <v>1</v>
       </c>
       <c r="D150" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E150">
-        <v>780</v>
+        <v>5779</v>
       </c>
       <c r="F150">
-        <v>780</v>
+        <v>5779</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -3950,27 +3944,27 @@
         <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E151">
-        <v>5779</v>
+        <v>6152</v>
       </c>
       <c r="F151">
-        <v>5779</v>
+        <v>6152</v>
       </c>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B152">
         <v>12000</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E152">
         <v>6152</v>
@@ -3981,16 +3975,16 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B153">
         <v>12000</v>
       </c>
       <c r="C153">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D153" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E153">
         <v>6152</v>
@@ -4001,16 +3995,16 @@
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B154">
         <v>12000</v>
       </c>
       <c r="C154">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D154" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E154">
         <v>6152</v>
@@ -4021,36 +4015,36 @@
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B155">
         <v>12000</v>
       </c>
       <c r="C155">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D155" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E155">
-        <v>6152</v>
+        <v>11730</v>
       </c>
       <c r="F155">
-        <v>6152</v>
+        <v>11730</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B156">
         <v>12000</v>
       </c>
       <c r="C156">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E156">
         <v>11730</v>
@@ -4061,202 +4055,202 @@
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B157">
         <v>12000</v>
       </c>
       <c r="C157">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D157" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E157">
-        <v>11730</v>
+        <v>11427</v>
       </c>
       <c r="F157">
-        <v>11730</v>
+        <v>11427</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B158">
         <v>12000</v>
       </c>
       <c r="C158">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D158" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E158">
-        <v>11427</v>
+        <v>11139</v>
       </c>
       <c r="F158">
-        <v>11427</v>
+        <v>11139</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B159">
         <v>12000</v>
       </c>
       <c r="C159">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D159" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E159">
-        <v>11139</v>
+        <v>10343</v>
       </c>
       <c r="F159">
-        <v>11139</v>
+        <v>10343</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B160">
         <v>12000</v>
       </c>
       <c r="C160">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D160" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E160">
-        <v>10343</v>
+        <v>11919</v>
       </c>
       <c r="F160">
-        <v>10343</v>
+        <v>11919</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B161">
         <v>12000</v>
       </c>
       <c r="C161">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D161" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E161">
-        <v>11919</v>
+        <v>11442</v>
       </c>
       <c r="F161">
-        <v>11919</v>
+        <v>11442</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B162">
         <v>12000</v>
       </c>
       <c r="C162">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D162" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E162">
-        <v>11442</v>
+        <v>11185</v>
       </c>
       <c r="F162">
-        <v>11442</v>
+        <v>11185</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B163">
         <v>12000</v>
       </c>
       <c r="C163">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D163" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E163">
-        <v>11185</v>
+        <v>10410</v>
       </c>
       <c r="F163">
-        <v>11185</v>
+        <v>10410</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B164">
         <v>12000</v>
       </c>
       <c r="C164">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D164" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E164">
-        <v>10410</v>
+        <v>10998</v>
       </c>
       <c r="F164">
-        <v>10410</v>
+        <v>10998</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B165">
         <v>12000</v>
       </c>
       <c r="C165">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D165" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E165">
-        <v>10998</v>
+        <v>10617</v>
       </c>
       <c r="F165">
-        <v>10998</v>
+        <v>10617</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B166">
         <v>12000</v>
       </c>
       <c r="C166">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D166" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E166">
-        <v>10617</v>
+        <v>5253</v>
       </c>
       <c r="F166">
-        <v>10617</v>
+        <v>5253</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -4267,75 +4261,55 @@
         <v>12000</v>
       </c>
       <c r="C167">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E167">
-        <v>5253</v>
+        <v>10314</v>
       </c>
       <c r="F167">
-        <v>5253</v>
+        <v>10314</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B168">
         <v>12000</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D168" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E168">
-        <v>10314</v>
+        <v>11723</v>
       </c>
       <c r="F168">
-        <v>10314</v>
+        <v>11723</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B169">
         <v>12000</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D169" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E169">
-        <v>11723</v>
+        <v>4800</v>
       </c>
       <c r="F169">
-        <v>11723</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="A170" t="s">
-        <v>69</v>
-      </c>
-      <c r="B170">
-        <v>12000</v>
-      </c>
-      <c r="C170">
-        <v>3</v>
-      </c>
-      <c r="D170" t="s">
-        <v>172</v>
-      </c>
-      <c r="E170">
-        <v>4800</v>
-      </c>
-      <c r="F170">
         <v>4800</v>
       </c>
     </row>

</xml_diff>